<commit_message>
css for search bar
</commit_message>
<xml_diff>
--- a/imaging_system_app_project/static/excel/ExcelDatabase.xlsx
+++ b/imaging_system_app_project/static/excel/ExcelDatabase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
   <si>
     <t>cust_id</t>
   </si>
@@ -44,15 +44,18 @@
     <t>One Company</t>
   </si>
   <si>
+    <t>44734567890</t>
+  </si>
+  <si>
+    <t>One@dummy-mail.com</t>
+  </si>
+  <si>
+    <t>Company Two</t>
+  </si>
+  <si>
     <t>44734567891</t>
   </si>
   <si>
-    <t>One@dummy-mail.com</t>
-  </si>
-  <si>
-    <t>Company Two</t>
-  </si>
-  <si>
     <t>CompanyTwo@dummy-mail.com</t>
   </si>
   <si>
@@ -237,6 +240,12 @@
   </si>
   <si>
     <t>Cryopreparation: LR white</t>
+  </si>
+  <si>
+    <t>JEOL 6000</t>
+  </si>
+  <si>
+    <t>JEOL 10000</t>
   </si>
   <si>
     <t>worker_id</t>
@@ -736,10 +745,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>103</v>
@@ -753,13 +762,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>112</v>
@@ -773,13 +782,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>105</v>
@@ -793,13 +802,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>121</v>
@@ -813,13 +822,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>116</v>
@@ -843,76 +852,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -920,16 +929,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -940,7 +949,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -960,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -969,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="W4">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -980,7 +989,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1000,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -1020,7 +1029,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -1042,7 +1051,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1050,22 +1059,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1073,19 +1082,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E2">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1093,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3">
         <v>55</v>
@@ -1105,7 +1114,7 @@
         <v>82.5</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1113,7 +1122,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -1125,7 +1134,7 @@
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1133,7 +1142,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -1145,7 +1154,7 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1153,7 +1162,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -1165,7 +1174,7 @@
         <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1173,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1185,7 +1194,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1193,7 +1202,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1205,7 +1214,7 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1213,7 +1222,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9">
         <v>200</v>
@@ -1225,7 +1234,7 @@
         <v>300</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1233,7 +1242,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -1245,7 +1254,7 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1253,7 +1262,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C11">
         <v>70</v>
@@ -1265,7 +1274,7 @@
         <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1273,7 +1282,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C12">
         <v>150</v>
@@ -1285,7 +1294,7 @@
         <v>225</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1293,7 +1302,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -1305,7 +1314,7 @@
         <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1313,7 +1322,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C14">
         <v>80</v>
@@ -1325,7 +1334,47 @@
         <v>120</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>35</v>
+      </c>
+      <c r="E15">
+        <v>105</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>150</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1343,19 +1392,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1363,13 +1412,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1380,13 +1429,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1397,13 +1446,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1414,13 +1463,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1431,13 +1480,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1448,13 +1497,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1475,13 +1524,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1576,19 +1625,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1599,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1633,7 +1682,7 @@
         <v>1.5</v>
       </c>
       <c r="C4">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1742,13 +1791,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1832,31 +1881,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1864,19 +1913,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H2">
-        <v>490</v>
+        <v>585</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1887,10 +1936,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H3">
         <v>292.5</v>

</xml_diff>

<commit_message>
fix: Use STATIC_ROOT, requires moving static files to new directories
</commit_message>
<xml_diff>
--- a/imaging_system_app_project/static/excel/ExcelDatabase.xlsx
+++ b/imaging_system_app_project/static/excel/ExcelDatabase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
   <si>
     <t>cust_id</t>
   </si>
@@ -41,43 +41,40 @@
     <t>cust_type</t>
   </si>
   <si>
-    <t>One Company</t>
-  </si>
-  <si>
-    <t>44734567890</t>
+    <t>Sample Company 1</t>
+  </si>
+  <si>
+    <t>44734567891</t>
   </si>
   <si>
     <t>One@dummy-mail.com</t>
   </si>
   <si>
-    <t>Company Two</t>
-  </si>
-  <si>
-    <t>44734567891</t>
+    <t>Sample Company 2</t>
   </si>
   <si>
     <t>CompanyTwo@dummy-mail.com</t>
   </si>
   <si>
-    <t>Third Company</t>
+    <t>Sample Company 3</t>
   </si>
   <si>
     <t>ThirdC@dummy-mail.com</t>
   </si>
   <si>
-    <t>4Company</t>
+    <t>Sample Company 4</t>
   </si>
   <si>
     <t>4company@dummy-mail.com</t>
   </si>
   <si>
-    <t>FiveGuys Burger</t>
+    <t>Sample Company 5</t>
   </si>
   <si>
     <t>FiveGuys@dummy-mail.com</t>
   </si>
   <si>
-    <t>6th and Co.</t>
+    <t>Sample Company 6</t>
   </si>
   <si>
     <t>6andCo@dummy-mail.com</t>
@@ -242,12 +239,6 @@
     <t>Cryopreparation: LR white</t>
   </si>
   <si>
-    <t>JEOL 6000</t>
-  </si>
-  <si>
-    <t>JEOL 10000</t>
-  </si>
-  <si>
     <t>worker_id</t>
   </si>
   <si>
@@ -360,6 +351,12 @@
   </si>
   <si>
     <t>111, DumDum street, Dum City</t>
+  </si>
+  <si>
+    <t>Sample extra 1</t>
+  </si>
+  <si>
+    <t>Sample extra 2</t>
   </si>
 </sst>
 </file>
@@ -745,10 +742,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
       <c r="E3">
         <v>103</v>
@@ -762,13 +759,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
       <c r="E4">
         <v>112</v>
@@ -782,13 +779,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
       <c r="E5">
         <v>105</v>
@@ -802,13 +799,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
       <c r="E6">
         <v>121</v>
@@ -822,13 +819,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
       </c>
       <c r="E7">
         <v>116</v>
@@ -852,76 +849,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>41</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>42</v>
-      </c>
-      <c r="X1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -929,16 +926,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -949,7 +946,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -969,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -978,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="W4">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -989,7 +986,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1009,7 +1006,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -1029,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -1051,7 +1048,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1059,22 +1056,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1082,19 +1079,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
         <v>56</v>
-      </c>
-      <c r="C2">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <v>40</v>
-      </c>
-      <c r="E2">
-        <v>120</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1102,7 +1099,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>55</v>
@@ -1114,7 +1111,7 @@
         <v>82.5</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1122,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -1134,7 +1131,7 @@
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1142,7 +1139,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -1154,7 +1151,7 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1162,7 +1159,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -1174,7 +1171,7 @@
         <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1182,7 +1179,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1194,7 +1191,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1202,7 +1199,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1214,7 +1211,7 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1222,7 +1219,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>200</v>
@@ -1234,7 +1231,7 @@
         <v>300</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1242,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -1254,7 +1251,7 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1262,7 +1259,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>70</v>
@@ -1274,7 +1271,7 @@
         <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1282,7 +1279,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12">
         <v>150</v>
@@ -1294,7 +1291,7 @@
         <v>225</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1302,7 +1299,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -1314,7 +1311,7 @@
         <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1322,7 +1319,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14">
         <v>80</v>
@@ -1334,47 +1331,7 @@
         <v>120</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15">
-        <v>70</v>
-      </c>
-      <c r="D15">
-        <v>35</v>
-      </c>
-      <c r="E15">
-        <v>105</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-      <c r="D16">
-        <v>50</v>
-      </c>
-      <c r="E16">
-        <v>150</v>
-      </c>
-      <c r="F16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1392,19 +1349,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1412,13 +1369,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1429,13 +1386,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1446,13 +1403,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1463,13 +1420,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1480,13 +1437,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1497,13 +1454,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1524,13 +1481,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1590,24 +1547,24 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1625,19 +1582,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1648,7 +1605,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1682,7 +1639,7 @@
         <v>1.5</v>
       </c>
       <c r="C4">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1791,13 +1748,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1881,31 +1838,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>103</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>104</v>
       </c>
-      <c r="F1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" t="s">
-        <v>107</v>
-      </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1913,19 +1870,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="H2">
-        <v>585</v>
+        <v>490</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1936,13 +1893,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>111</v>
       </c>
-      <c r="C3" t="s">
-        <v>112</v>
+      <c r="G3">
+        <v>20</v>
       </c>
       <c r="H3">
-        <v>292.5</v>
+        <v>322.5</v>
       </c>
       <c r="I3">
         <v>2</v>

</xml_diff>